<commit_message>
Include: Stripe to Payment Gateway Comparison Matrix
</commit_message>
<xml_diff>
--- a/Semester-2/Innovation-Project-Pt2/Supporting-Documents/Gateway-Comparison.xlsx
+++ b/Semester-2/Innovation-Project-Pt2/Supporting-Documents/Gateway-Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\TAFE\Dual-Diploma-2024\Semester-2\Innovation-Project-Pt2\Supporting-Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA074559-1652-44FB-AB3B-AA3C87C44A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9252C2B-0D24-4300-BA84-2EBC36924EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{75D1E102-0EAF-4376-8D2F-F3C45DF2388F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Payment Gatway Comparison Matrix</t>
   </si>
@@ -104,20 +104,113 @@
     <t>None</t>
   </si>
   <si>
-    <t>Credit/Debit cards &amp; Direct Debit</t>
-  </si>
-  <si>
-    <t>PCI-DSS compliant, fraud prevention tools</t>
-  </si>
-  <si>
-    <t>API</t>
+    <t>YES [flutter_stripe]</t>
+  </si>
+  <si>
+    <t>3.5% + A$0.30 [International]</t>
+  </si>
+  <si>
+    <t>1. PCI-DSS compliant</t>
+  </si>
+  <si>
+    <t>1. FDIC insurance</t>
+  </si>
+  <si>
+    <t>2. Encryption ( AES-256)</t>
+  </si>
+  <si>
+    <t>3. Tokenisation</t>
+  </si>
+  <si>
+    <t>4. Penetration Testing</t>
+  </si>
+  <si>
+    <t>5. Provider’s registration</t>
+  </si>
+  <si>
+    <t>6. SSL (or TLS) + HTTPS Communication</t>
+  </si>
+  <si>
+    <t>7.PCI-DSS compliant (PCI Service Provider - Level 1)</t>
+  </si>
+  <si>
+    <t>8. Bug Bounties</t>
+  </si>
+  <si>
+    <t>9. Supports 2FA</t>
+  </si>
+  <si>
+    <t>1.BankTransfers.</t>
+  </si>
+  <si>
+    <t>2.BankRedirect.</t>
+  </si>
+  <si>
+    <t>3.Buy-now-pay later.</t>
+  </si>
+  <si>
+    <t>4.Cards.</t>
+  </si>
+  <si>
+    <t>5.Real-time-payments.</t>
+  </si>
+  <si>
+    <t>6.Wallets.</t>
+  </si>
+  <si>
+    <t>7.Cash-based-voucher.</t>
+  </si>
+  <si>
+    <t>8.Bank-Debits.</t>
+  </si>
+  <si>
+    <t>2. Direct Debit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Credit/Debit cards </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Standard: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.7% + A$0.30 [Domestic]</t>
+    </r>
+  </si>
+  <si>
+    <t>2. E-commerce extensions</t>
+  </si>
+  <si>
+    <t>1. API</t>
+  </si>
+  <si>
+    <t>2. Fraud prevention tools</t>
+  </si>
+  <si>
+    <t>24hr Support</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,8 +255,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,8 +314,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -264,20 +396,256 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -293,9 +661,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -305,8 +670,129 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -644,16 +1130,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF8A19E-1F8D-43D2-BC89-FFE87DF1F7F5}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30" style="21" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
@@ -662,196 +1149,469 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="34.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="9"/>
+      <c r="A1" s="8"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="8"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" s="15" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="1:10" s="13" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="14"/>
-    </row>
-    <row r="5" spans="1:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="C4" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="10"/>
-    </row>
-    <row r="6" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="C5" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="10"/>
-    </row>
-    <row r="7" spans="1:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="C7" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="10"/>
-    </row>
-    <row r="8" spans="1:10" ht="57" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="B8" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
+      <c r="B12" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="18"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="10"/>
-    </row>
-    <row r="9" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="B16" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="1:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="9"/>
+    </row>
+    <row r="22" spans="1:10" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="9"/>
+    </row>
+    <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="9"/>
+    </row>
+    <row r="24" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="18"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="9"/>
+    </row>
+    <row r="25" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="10"/>
-    </row>
-    <row r="10" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="B25" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="9"/>
+    </row>
+    <row r="26" spans="1:10" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="16"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="9"/>
+    </row>
+    <row r="27" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B27" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="10"/>
-    </row>
-    <row r="11" spans="1:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="C27" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="9"/>
+    </row>
+    <row r="28" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B28" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
+      <c r="C28" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="9"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="8"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A16:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="A8:A15"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{9B7D17B2-0389-4DA3-82CC-53FC51AF56C5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>